<commit_message>
added tests for reading PDF + adjusted test for working with xlsx
</commit_message>
<xml_diff>
--- a/Excel01.xlsx
+++ b/Excel01.xlsx
@@ -1,60 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PyCharm_Projects_2\RF_1\rf1\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DAB4AD-20E8-4129-80DA-854A574ED4C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1860" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -73,21 +46,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -353,29 +317,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>